<commit_message>
[Solved] Comment Issuegit add .
</commit_message>
<xml_diff>
--- a/Course-Progress.xlsx
+++ b/Course-Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gain-Insights\InfoXD\react-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F51022-CE3D-49DF-8084-40A836118AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB54A878-35E8-4961-96EB-388DB03065EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,12 @@
 https://github.com/JayrajShah/react-course-gi/tree/master/app-13_1
 App Link:
 https://react-http-48387.web.app/</t>
+  </si>
+  <si>
+    <t>Authentication App: Firebase Authentication
+React Router: Protected Routes
+App-14
+https://github.com/JayrajShah/react-course-gi/tree/master/app-14</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,8 +571,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44371</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>